<commit_message>
`Added new options to dropdown menus in various PHP files`
</commit_message>
<xml_diff>
--- a/web/assets/Format.xlsx
+++ b/web/assets/Format.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fajrul\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F6AD52F-4C2E-4D5C-992B-660C1593EE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D00202-2643-4D6A-B92E-B5262FA49732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5FAFC18C-40CF-44BB-9798-1FC9E1B2BDF9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Order_ID</t>
   </si>
@@ -43,13 +43,91 @@
   </si>
   <si>
     <t>Order_By</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>INDIHOME</t>
+  </si>
+  <si>
+    <t>Order ke 1</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Plasa</t>
+  </si>
+  <si>
+    <t>WO0123590</t>
+  </si>
+  <si>
+    <t>Order ke 2</t>
+  </si>
+  <si>
+    <t>WO0123591</t>
+  </si>
+  <si>
+    <t>Order ke 3</t>
+  </si>
+  <si>
+    <t>WO0123592</t>
+  </si>
+  <si>
+    <t>Order ke 4</t>
+  </si>
+  <si>
+    <t>WO0123593</t>
+  </si>
+  <si>
+    <t>Order ke 5</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>INDIBIZ</t>
+  </si>
+  <si>
+    <t>Teknisi</t>
+  </si>
+  <si>
+    <t>WO0123594</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>Pickup</t>
+  </si>
+  <si>
+    <t>WIFIID</t>
+  </si>
+  <si>
+    <t>PSB</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>OLO</t>
+  </si>
+  <si>
+    <t>PDA</t>
+  </si>
+  <si>
+    <t>VPNIP</t>
+  </si>
+  <si>
+    <t>CLose</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,16 +135,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -74,12 +164,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,38 +501,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0700D247-33F0-40F1-8D52-FCB496E456DD}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>